<commit_message>
Actualización Procedimientos de Pensiones a Ascci
</commit_message>
<xml_diff>
--- a/senosiain/Horas/horas-quincena 2 Julio 2025.xlsx
+++ b/senosiain/Horas/horas-quincena 2 Julio 2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Terceros\fortia\Senosiain\Horas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B8E02-7F0B-49D1-8EBD-550158A58395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0562B4-1994-4DBA-8069-A755F6D5F911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>fecha</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Saldo</t>
-  </si>
-  <si>
-    <t>2da Quincena Julio 2025</t>
   </si>
   <si>
     <t>Junta de Análisis de requerimiento extracción Firma trabajadores</t>
@@ -109,6 +106,27 @@
   </si>
   <si>
     <t>Actualización procedimiento splseGenLinBanamexPensiones2024 (Generación de Archivo de pensiones)</t>
+  </si>
+  <si>
+    <t>11:00:00 a.m.</t>
+  </si>
+  <si>
+    <t>11:30:00 a.m.</t>
+  </si>
+  <si>
+    <t>Abono a cuenta</t>
+  </si>
+  <si>
+    <t>01:00:00 p.m.</t>
+  </si>
+  <si>
+    <t>02:00:00 p.m.</t>
+  </si>
+  <si>
+    <t>Presentación de la clave del banco cuando el proceso es interbancario en  procedimiento splseGenLinBanamexPensiones2024</t>
+  </si>
+  <si>
+    <t>2da Quincena Agosto 2025</t>
   </si>
 </sst>
 </file>
@@ -234,13 +252,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -294,7 +312,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:E11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:E12">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="fecha" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora Inicio"/>
@@ -504,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H995"/>
+  <dimension ref="A1:H996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -515,20 +533,20 @@
     <col min="1" max="1" width="14" style="11" customWidth="1"/>
     <col min="2" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="12.08984375" customWidth="1"/>
-    <col min="5" max="5" width="99" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.90625" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" customWidth="1"/>
     <col min="7" max="7" width="33.7265625" customWidth="1"/>
     <col min="8" max="8" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="A1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
@@ -548,8 +566,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18" t="s">
-        <v>11</v>
+      <c r="A3" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -557,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="5"/>
     </row>
@@ -565,25 +583,25 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="E4" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -591,16 +609,16 @@
         <v>45874</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -608,7 +626,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -616,76 +634,108 @@
         <v>45875</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="15">
+        <v>45876</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="15">
+        <v>45883</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="8">
-        <f>SUBTOTAL(109,D3:D10)</f>
-        <v>7</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="13">
-        <f>+D11*500</f>
-        <v>3500</v>
-      </c>
+    <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <f>SUBTOTAL(109,D3:D11)</f>
+        <v>8</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="14"/>
+    <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="13">
+        <f>+D12*500</f>
+        <v>4000</v>
+      </c>
     </row>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="14"/>
+      <c r="A16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="14">
+        <v>3000</v>
+      </c>
     </row>
     <row r="17" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="14">
-        <f>+D13-D15</f>
-        <v>3500</v>
+      <c r="D18" s="14">
+        <f>+D14-D16</f>
+        <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="3:4" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="3:4" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="3:4" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="28" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -874,7 +924,7 @@
     <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1654,6 +1704,7 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>